<commit_message>
first commit offline mode
</commit_message>
<xml_diff>
--- a/xls_folder/adaptacion_emision_boletos.xlsx
+++ b/xls_folder/adaptacion_emision_boletos.xlsx
@@ -8,15 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario.diaz.rodriguez\PycharmProjects\CitiBank_Boletos\xls_folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{646BE6EC-63A1-4C5D-A0DD-009BFD0AD82D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB3BB57-98F4-4600-9A88-79A9F9EEE251}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -25,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="34">
   <si>
     <r>
       <rPr>
@@ -198,6 +204,21 @@
   </si>
   <si>
     <t>Payer Zip Code</t>
+  </si>
+  <si>
+    <t>test1 S/A</t>
+  </si>
+  <si>
+    <t>ñoqui</t>
+  </si>
+  <si>
+    <t>ácéntú</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0453</t>
+  </si>
+  <si>
+    <t>6666</t>
   </si>
 </sst>
 </file>
@@ -290,7 +311,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -306,7 +327,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -693,23 +713,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P22"/>
+  <dimension ref="A1:P43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="50.28515625" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1"/>
     <col min="4" max="4" width="52.85546875" customWidth="1"/>
     <col min="5" max="5" width="12.140625" customWidth="1"/>
     <col min="6" max="6" width="36.85546875" customWidth="1"/>
     <col min="7" max="7" width="79.7109375" customWidth="1"/>
     <col min="8" max="8" width="8.7109375" customWidth="1"/>
-    <col min="9" max="9" width="20.7109375" style="11" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" style="10" customWidth="1"/>
     <col min="10" max="10" width="30.5703125" customWidth="1"/>
     <col min="11" max="11" width="15.7109375" customWidth="1"/>
     <col min="12" max="12" width="17" customWidth="1"/>
@@ -739,25 +759,25 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="M1" s="9" t="s">
         <v>28</v>
       </c>
       <c r="N1" s="3" t="s">
@@ -772,14 +792,14 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
-        <v>54947</v>
+        <v>66666</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D2" s="4">
-        <v>30306294000226</v>
+        <v>1</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="5">
@@ -791,7 +811,7 @@
       <c r="H2">
         <v>100</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="10" t="s">
         <v>20</v>
       </c>
       <c r="J2" t="s">
@@ -803,7 +823,7 @@
       <c r="L2" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="11" t="s">
+      <c r="M2" s="10" t="s">
         <v>17</v>
       </c>
       <c r="N2" s="6" t="s">
@@ -813,19 +833,19 @@
         <v>13</v>
       </c>
       <c r="P2" s="8">
-        <v>26875.31</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
-        <v>54948</v>
+        <v>66667</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="D3" s="4">
-        <v>30306294000226</v>
+        <v>123456789</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="5">
@@ -837,7 +857,7 @@
       <c r="H3">
         <v>180</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="I3" s="10" t="s">
         <v>21</v>
       </c>
       <c r="J3" t="s">
@@ -849,8 +869,8 @@
       <c r="L3" t="s">
         <v>18</v>
       </c>
-      <c r="M3" s="11" t="s">
-        <v>23</v>
+      <c r="M3" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="N3" s="6" t="s">
         <v>12</v>
@@ -859,19 +879,19 @@
         <v>13</v>
       </c>
       <c r="P3" s="8">
-        <v>59021.68</v>
+        <v>10001</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
-        <v>54949</v>
+        <v>66668</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="D4" s="4">
-        <v>30306294000226</v>
+        <v>226</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="5">
@@ -883,7 +903,7 @@
       <c r="H4">
         <v>100</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="10" t="s">
         <v>22</v>
       </c>
       <c r="J4" t="s">
@@ -895,8 +915,8 @@
       <c r="L4" t="s">
         <v>18</v>
       </c>
-      <c r="M4" s="11" t="s">
-        <v>24</v>
+      <c r="M4" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="N4" s="6" t="s">
         <v>12</v>
@@ -905,44 +925,146 @@
         <v>13</v>
       </c>
       <c r="P4" s="8">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>54947</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="4">
+        <v>30306294000226</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="5">
+        <v>96534094000158</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5">
+        <v>100</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="O5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="P5" s="8">
+        <v>26875.31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>54948</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="4">
+        <v>30306294000226</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="5">
+        <v>96534094000158</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6">
+        <v>180</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M6" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="O6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="P6" s="8">
+        <v>59021.68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>54949</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="4">
+        <v>30306294000226</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="5">
+        <v>96534094000158</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7">
+        <v>100</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" t="s">
+        <v>16</v>
+      </c>
+      <c r="K7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L7" t="s">
+        <v>18</v>
+      </c>
+      <c r="M7" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="N7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="O7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="P7" s="8">
         <v>24122.23</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="4"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="4"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="4"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
@@ -950,11 +1072,12 @@
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
+      <c r="F8" s="5"/>
       <c r="G8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="4"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="8"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
@@ -962,11 +1085,12 @@
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
+      <c r="F9" s="5"/>
       <c r="G9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="9"/>
-      <c r="P9" s="4"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="8"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
@@ -974,11 +1098,12 @@
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
+      <c r="F10" s="5"/>
       <c r="G10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="4"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="8"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
@@ -986,11 +1111,12 @@
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
+      <c r="F11" s="5"/>
       <c r="G11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="9"/>
-      <c r="P11" s="4"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="8"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
@@ -998,11 +1124,12 @@
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
+      <c r="F12" s="5"/>
       <c r="G12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="4"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="8"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
@@ -1010,11 +1137,12 @@
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
+      <c r="F13" s="5"/>
       <c r="G13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="4"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="8"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
@@ -1022,11 +1150,12 @@
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
+      <c r="F14" s="5"/>
       <c r="G14" s="4"/>
-      <c r="N14" s="4"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="4"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="8"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
@@ -1034,11 +1163,12 @@
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
+      <c r="F15" s="5"/>
       <c r="G15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="9"/>
-      <c r="P15" s="4"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="8"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
@@ -1046,11 +1176,12 @@
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
+      <c r="F16" s="5"/>
       <c r="G16" s="4"/>
-      <c r="N16" s="4"/>
-      <c r="O16" s="9"/>
-      <c r="P16" s="4"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="8"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
@@ -1058,11 +1189,12 @@
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
+      <c r="F17" s="5"/>
       <c r="G17" s="4"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="9"/>
-      <c r="P17" s="4"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="8"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
@@ -1070,11 +1202,12 @@
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
+      <c r="F18" s="5"/>
       <c r="G18" s="4"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="9"/>
-      <c r="P18" s="4"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="8"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
@@ -1082,11 +1215,12 @@
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
+      <c r="F19" s="5"/>
       <c r="G19" s="4"/>
-      <c r="N19" s="4"/>
-      <c r="O19" s="9"/>
-      <c r="P19" s="4"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="8"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
@@ -1094,11 +1228,12 @@
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
+      <c r="F20" s="5"/>
       <c r="G20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="9"/>
-      <c r="P20" s="4"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="8"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
@@ -1106,11 +1241,12 @@
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
+      <c r="F21" s="5"/>
       <c r="G21" s="4"/>
-      <c r="N21" s="4"/>
-      <c r="O21" s="9"/>
-      <c r="P21" s="4"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="8"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
@@ -1118,11 +1254,285 @@
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
+      <c r="F22" s="5"/>
       <c r="G22" s="4"/>
-      <c r="N22" s="4"/>
-      <c r="O22" s="9"/>
-      <c r="P22" s="4"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="7"/>
+      <c r="P22" s="8"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="4"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="7"/>
+      <c r="P23" s="8"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="4"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="8"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="4"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="6"/>
+      <c r="O25" s="7"/>
+      <c r="P25" s="8"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="4"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="6"/>
+      <c r="O26" s="7"/>
+      <c r="P26" s="8"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="4"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="6"/>
+      <c r="O27" s="7"/>
+      <c r="P27" s="8"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="4"/>
+      <c r="M28" s="10"/>
+      <c r="N28" s="6"/>
+      <c r="O28" s="7"/>
+      <c r="P28" s="8"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="4"/>
+      <c r="M29" s="10"/>
+      <c r="N29" s="6"/>
+      <c r="O29" s="7"/>
+      <c r="P29" s="8"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="4"/>
+      <c r="M30" s="10"/>
+      <c r="N30" s="6"/>
+      <c r="O30" s="7"/>
+      <c r="P30" s="8"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="4"/>
+      <c r="M31" s="10"/>
+      <c r="N31" s="6"/>
+      <c r="O31" s="7"/>
+      <c r="P31" s="8"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="4"/>
+      <c r="M32" s="10"/>
+      <c r="N32" s="6"/>
+      <c r="O32" s="7"/>
+      <c r="P32" s="8"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="4"/>
+      <c r="M33" s="10"/>
+      <c r="N33" s="6"/>
+      <c r="O33" s="7"/>
+      <c r="P33" s="8"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="4"/>
+      <c r="M34" s="10"/>
+      <c r="N34" s="6"/>
+      <c r="O34" s="7"/>
+      <c r="P34" s="8"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="4"/>
+      <c r="M35" s="10"/>
+      <c r="N35" s="6"/>
+      <c r="O35" s="7"/>
+      <c r="P35" s="8"/>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="4"/>
+      <c r="M36" s="10"/>
+      <c r="N36" s="6"/>
+      <c r="O36" s="7"/>
+      <c r="P36" s="8"/>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="4"/>
+      <c r="M37" s="10"/>
+      <c r="N37" s="6"/>
+      <c r="O37" s="7"/>
+      <c r="P37" s="8"/>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="4"/>
+      <c r="M38" s="10"/>
+      <c r="N38" s="6"/>
+      <c r="O38" s="7"/>
+      <c r="P38" s="8"/>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="4"/>
+      <c r="M39" s="10"/>
+      <c r="N39" s="6"/>
+      <c r="O39" s="7"/>
+      <c r="P39" s="8"/>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="4"/>
+      <c r="M40" s="10"/>
+      <c r="N40" s="6"/>
+      <c r="O40" s="7"/>
+      <c r="P40" s="8"/>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="4"/>
+      <c r="M41" s="10"/>
+      <c r="N41" s="6"/>
+      <c r="O41" s="7"/>
+      <c r="P41" s="8"/>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="4"/>
+      <c r="M42" s="10"/>
+      <c r="N42" s="6"/>
+      <c r="O42" s="7"/>
+      <c r="P42" s="8"/>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="4"/>
+      <c r="M43" s="10"/>
+      <c r="N43" s="6"/>
+      <c r="O43" s="7"/>
+      <c r="P43" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
se contemplan y capturan errores en la generacion del boleto
</commit_message>
<xml_diff>
--- a/xls_folder/adaptacion_emision_boletos.xlsx
+++ b/xls_folder/adaptacion_emision_boletos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario.diaz.rodriguez\PycharmProjects\CitiBank_Boletos\xls_folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB3BB57-98F4-4600-9A88-79A9F9EEE251}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C9DF5F4-6EDF-4B9C-9FD6-DCC59F24792F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="33">
   <si>
     <r>
       <rPr>
@@ -204,9 +204,6 @@
   </si>
   <si>
     <t>Payer Zip Code</t>
-  </si>
-  <si>
-    <t>test1 S/A</t>
   </si>
   <si>
     <t>ñoqui</t>
@@ -716,7 +713,7 @@
   <dimension ref="A1:P43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD45"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -795,9 +792,7 @@
         <v>66666</v>
       </c>
       <c r="B2" s="4"/>
-      <c r="C2" s="4" t="s">
-        <v>29</v>
-      </c>
+      <c r="C2" s="4"/>
       <c r="D2" s="4">
         <v>1</v>
       </c>
@@ -842,7 +837,7 @@
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D3" s="4">
         <v>123456789</v>
@@ -870,7 +865,7 @@
         <v>18</v>
       </c>
       <c r="M3" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N3" s="6" t="s">
         <v>12</v>
@@ -888,7 +883,7 @@
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" s="4">
         <v>226</v>
@@ -916,7 +911,7 @@
         <v>18</v>
       </c>
       <c r="M4" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N4" s="6" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
seems to be fine
</commit_message>
<xml_diff>
--- a/xls_folder/adaptacion_emision_boletos.xlsx
+++ b/xls_folder/adaptacion_emision_boletos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario.diaz.rodriguez\PycharmProjects\CitiBank_Boletos\xls_folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C9DF5F4-6EDF-4B9C-9FD6-DCC59F24792F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{363112F9-F3BD-4C61-A6BD-5121EDDFF0B1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="44">
   <si>
     <r>
       <rPr>
@@ -155,12 +155,6 @@
     <t>AV BRIGADEIRO FARIA LIMA 3477. CEP: 04538133. SAO PAULO. SP</t>
   </si>
   <si>
-    <t>13/09/2019</t>
-  </si>
-  <si>
-    <t>30/09/2019</t>
-  </si>
-  <si>
     <t>Product</t>
   </si>
   <si>
@@ -216,6 +210,45 @@
   </si>
   <si>
     <t>6666</t>
+  </si>
+  <si>
+    <t>09/13/2019</t>
+  </si>
+  <si>
+    <t>09/13/2020</t>
+  </si>
+  <si>
+    <t>09/13/2021</t>
+  </si>
+  <si>
+    <t>09/13/2022</t>
+  </si>
+  <si>
+    <t>09/13/2023</t>
+  </si>
+  <si>
+    <t>09/13/2024</t>
+  </si>
+  <si>
+    <t>09/30/2019</t>
+  </si>
+  <si>
+    <t>09/30/2020</t>
+  </si>
+  <si>
+    <t>09/30/2021</t>
+  </si>
+  <si>
+    <t>09/30/2022</t>
+  </si>
+  <si>
+    <t>09/30/2023</t>
+  </si>
+  <si>
+    <t>09/30/2024</t>
+  </si>
+  <si>
+    <t>02</t>
   </si>
 </sst>
 </file>
@@ -308,7 +341,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -328,6 +361,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -712,8 +748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,22 +796,22 @@
         <v>6</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J1" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="M1" s="9" t="s">
         <v>26</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>28</v>
       </c>
       <c r="N1" s="3" t="s">
         <v>7</v>
@@ -798,7 +834,7 @@
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="5">
-        <v>96534094000158</v>
+        <v>1</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>11</v>
@@ -807,25 +843,25 @@
         <v>100</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" t="s">
         <v>16</v>
       </c>
-      <c r="K2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" t="s">
-        <v>18</v>
-      </c>
       <c r="M2" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>12</v>
+        <v>43</v>
+      </c>
+      <c r="N2" s="13" t="s">
+        <v>31</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="P2" s="8">
         <v>2</v>
@@ -837,7 +873,7 @@
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D3" s="4">
         <v>123456789</v>
@@ -853,25 +889,25 @@
         <v>180</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" t="s">
         <v>16</v>
       </c>
-      <c r="K3" t="s">
-        <v>19</v>
-      </c>
-      <c r="L3" t="s">
-        <v>18</v>
-      </c>
       <c r="M3" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="N3" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="N3" s="6" t="s">
-        <v>12</v>
-      </c>
       <c r="O3" s="7" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="P3" s="8">
         <v>10001</v>
@@ -883,7 +919,7 @@
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D4" s="4">
         <v>226</v>
@@ -899,25 +935,25 @@
         <v>100</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" t="s">
         <v>16</v>
       </c>
-      <c r="K4" t="s">
-        <v>19</v>
-      </c>
-      <c r="L4" t="s">
-        <v>18</v>
-      </c>
       <c r="M4" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>12</v>
+        <v>29</v>
+      </c>
+      <c r="N4" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="O4" s="7" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="P4" s="8">
         <v>100000</v>
@@ -945,25 +981,25 @@
         <v>100</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L5" t="s">
         <v>16</v>
       </c>
-      <c r="K5" t="s">
-        <v>19</v>
-      </c>
-      <c r="L5" t="s">
-        <v>18</v>
-      </c>
       <c r="M5" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="N5" s="6" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="N5" s="13" t="s">
+        <v>34</v>
       </c>
       <c r="O5" s="7" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="P5" s="8">
         <v>26875.31</v>
@@ -991,25 +1027,25 @@
         <v>180</v>
       </c>
       <c r="I6" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" t="s">
+        <v>17</v>
+      </c>
+      <c r="L6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M6" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="J6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K6" t="s">
-        <v>19</v>
-      </c>
-      <c r="L6" t="s">
-        <v>18</v>
-      </c>
-      <c r="M6" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="N6" s="6" t="s">
-        <v>12</v>
+      <c r="N6" s="13" t="s">
+        <v>35</v>
       </c>
       <c r="O6" s="7" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="P6" s="8">
         <v>59021.68</v>
@@ -1037,25 +1073,25 @@
         <v>100</v>
       </c>
       <c r="I7" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" t="s">
+        <v>17</v>
+      </c>
+      <c r="L7" t="s">
+        <v>16</v>
+      </c>
+      <c r="M7" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="J7" t="s">
-        <v>16</v>
-      </c>
-      <c r="K7" t="s">
-        <v>19</v>
-      </c>
-      <c r="L7" t="s">
-        <v>18</v>
-      </c>
-      <c r="M7" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="N7" s="6" t="s">
-        <v>12</v>
+      <c r="N7" s="13" t="s">
+        <v>36</v>
       </c>
       <c r="O7" s="7" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="P7" s="8">
         <v>24122.23</v>
@@ -1148,7 +1184,7 @@
       <c r="F14" s="5"/>
       <c r="G14" s="4"/>
       <c r="M14" s="10"/>
-      <c r="N14" s="6"/>
+      <c r="N14" s="13"/>
       <c r="O14" s="7"/>
       <c r="P14" s="8"/>
     </row>

</xml_diff>